<commit_message>
Super fast code with proper OOP
</commit_message>
<xml_diff>
--- a/ReqPowDATA.xlsx
+++ b/ReqPowDATA.xlsx
@@ -502,64 +502,64 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>88.46478119038883</v>
+        <v>88.4545441393966</v>
       </c>
       <c r="C2" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="D2" t="n">
-        <v>1102.089876347605</v>
+        <v>1101.96296801947</v>
       </c>
       <c r="E2" t="n">
-        <v>1769.295623807777</v>
+        <v>1769.090882787932</v>
       </c>
       <c r="F2" t="n">
-        <v>1769.295623807777</v>
+        <v>1769.090882787932</v>
       </c>
       <c r="G2" t="n">
-        <v>1590.547993427122</v>
+        <v>1590.364055129905</v>
       </c>
       <c r="H2" t="n">
-        <v>1590.547993427122</v>
+        <v>1590.364055129905</v>
       </c>
       <c r="I2" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="J2" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="K2" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="L2" t="n">
-        <v>1769.295623807777</v>
+        <v>1769.090882787932</v>
       </c>
       <c r="M2" t="n">
-        <v>1769.295623807777</v>
+        <v>1769.090882787932</v>
       </c>
       <c r="N2" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="O2" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="P2" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="Q2" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="R2" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="S2" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="T2" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="U2" t="n">
-        <v>88.46478119038883</v>
+        <v>88.4545441393966</v>
       </c>
     </row>
     <row r="3">
@@ -569,64 +569,64 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>88.46478119038883</v>
+        <v>88.4545441393966</v>
       </c>
       <c r="C3" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="D3" t="n">
-        <v>886.6210818666552</v>
+        <v>886.5192438262889</v>
       </c>
       <c r="E3" t="n">
-        <v>1437.199606333079</v>
+        <v>1437.033505445532</v>
       </c>
       <c r="F3" t="n">
-        <v>1437.199606333079</v>
+        <v>1437.033505445532</v>
       </c>
       <c r="G3" t="n">
-        <v>1645.203938875824</v>
+        <v>1645.013641234165</v>
       </c>
       <c r="H3" t="n">
-        <v>1645.203938875824</v>
+        <v>1645.013641234165</v>
       </c>
       <c r="I3" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="J3" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="K3" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="L3" t="n">
-        <v>1437.199606333079</v>
+        <v>1437.033505445532</v>
       </c>
       <c r="M3" t="n">
-        <v>1437.199606333079</v>
+        <v>1437.033505445532</v>
       </c>
       <c r="N3" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="O3" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="P3" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="Q3" t="n">
-        <v>1485.165391385093</v>
+        <v>1484.992756861953</v>
       </c>
       <c r="R3" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="S3" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="T3" t="n">
-        <v>176.9295623807777</v>
+        <v>176.9090882787932</v>
       </c>
       <c r="U3" t="n">
-        <v>88.46478119038883</v>
+        <v>88.4545441393966</v>
       </c>
     </row>
     <row r="4">
@@ -642,19 +642,19 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>215.4687944809496</v>
+        <v>215.443724193181</v>
       </c>
       <c r="E4" t="n">
-        <v>332.0960174746977</v>
+        <v>332.0573773423994</v>
       </c>
       <c r="F4" t="n">
-        <v>332.0960174746977</v>
+        <v>332.0573773423994</v>
       </c>
       <c r="G4" t="n">
-        <v>-54.65594544870228</v>
+        <v>-54.64958610426001</v>
       </c>
       <c r="H4" t="n">
-        <v>-54.65594544870228</v>
+        <v>-54.64958610426001</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -666,10 +666,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>332.0960174746977</v>
+        <v>332.0573773423994</v>
       </c>
       <c r="M4" t="n">
-        <v>332.0960174746977</v>
+        <v>332.0573773423994</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>

</xml_diff>